<commit_message>
add staff login by phone number
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F39853-C1AC-4EBF-B80B-EAC54DA0B78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA7A2BC-6765-4466-984A-9BE95CFD9530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>email</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -546,6 +546,9 @@
       <c r="G2" s="1">
         <v>36980</v>
       </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
add refresh token & fix dob
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA7A2BC-6765-4466-984A-9BE95CFD9530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB021CA6-C395-4EFD-9712-8A06536FCB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>email</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/devnguvcl/public_hosting_image/main/img/100_31.jpg</t>
+  </si>
+  <si>
+    <t>2001-03-30</t>
   </si>
 </sst>
 </file>
@@ -183,12 +186,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +476,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -543,8 +546,8 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1">
-        <v>36980</v>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -555,7 +558,7 @@
       <c r="J2" t="b">
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -578,8 +581,8 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1">
-        <v>36994</v>
+      <c r="G3" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
@@ -590,7 +593,7 @@
       <c r="J3" t="b">
         <v>1</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -598,7 +601,7 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C4" t="s">
@@ -607,14 +610,14 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1">
-        <v>37150</v>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -625,7 +628,7 @@
       <c r="J4" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix dob mockup data
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB021CA6-C395-4EFD-9712-8A06536FCB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12583E3B-911C-49CD-9AF6-A74D65D61369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>email</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>2001-03-30</t>
+  </si>
+  <si>
+    <t>2001-04-13</t>
+  </si>
+  <si>
+    <t>2001-07-26</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -582,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
@@ -617,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
fix staff, user mockup data
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF512C2-FC87-4036-A2E0-4DB15FDB83EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7444E515-8905-4B6E-8047-A31A6D05C83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,9 +516,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="B21" sqref="A21:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,9 +1588,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{302FE3D0-BB18-404B-81DE-91BA2AA6FC90}"/>

</xml_diff>

<commit_message>
add mockup data staff cskh
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ABAEE3-B6D4-4593-B15E-85ADD8B5AB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D181906-BD71-4973-80C1-B57B4DC2E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="210">
   <si>
     <t>email</t>
   </si>
@@ -739,6 +739,45 @@
   </si>
   <si>
     <t>a12bc102-bab0-409e-9290-28320bea22ee</t>
+  </si>
+  <si>
+    <t>9edbd47a-186b-4c5b-a077-8446b7418f6f</t>
+  </si>
+  <si>
+    <t>2798c948-07a7-4f85-b7a6-8d8d69e53676</t>
+  </si>
+  <si>
+    <t>Customer_Service</t>
+  </si>
+  <si>
+    <t>xuanthanh@gmail.com</t>
+  </si>
+  <si>
+    <t>ngocnhu@gmail.com</t>
+  </si>
+  <si>
+    <t>0346494851</t>
+  </si>
+  <si>
+    <t>0366995813</t>
+  </si>
+  <si>
+    <t>Đỗ Xuân Thanh</t>
+  </si>
+  <si>
+    <t>Lê Ngọc Như</t>
+  </si>
+  <si>
+    <t>https://vapa.vn/wp-content/uploads/2022/12/anh-avatar-facebook-dep-001.jpg</t>
+  </si>
+  <si>
+    <t>https://thao68.com/wp-content/uploads/2022/03/avatar-facebook-3.jpg</t>
+  </si>
+  <si>
+    <t>xuanthanh</t>
+  </si>
+  <si>
+    <t>ngocnhu</t>
   </si>
 </sst>
 </file>
@@ -809,9 +848,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1094,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2083,6 +2123,94 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F22" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" t="s">
+        <v>206</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>161</v>
+      </c>
+      <c r="K22" t="s">
+        <v>109</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G23" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I23" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
merge nhu & format
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindonut\Documents\GitHub\Final\MEDRE_BE\src\models\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D1A9AB-9E1C-4D82-B293-AF16B53B3143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285E5614-4AF4-4085-8D80-1B07440413DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="211">
   <si>
     <t>email</t>
   </si>
@@ -748,6 +748,39 @@
   </si>
   <si>
     <t>transang123@gmail.com</t>
+  </si>
+  <si>
+    <t>9edbd47a-186b-4c5b-a077-8446b7418f6f</t>
+  </si>
+  <si>
+    <t>xuanthanh</t>
+  </si>
+  <si>
+    <t>Customer_Service</t>
+  </si>
+  <si>
+    <t>xuanthanh@gmail.com</t>
+  </si>
+  <si>
+    <t>Đỗ Xuân Thanh</t>
+  </si>
+  <si>
+    <t>https://vapa.vn/wp-content/uploads/2022/12/anh-avatar-facebook-dep-001.jpg</t>
+  </si>
+  <si>
+    <t>2798c948-07a7-4f85-b7a6-8d8d69e53676</t>
+  </si>
+  <si>
+    <t>ngocnhu</t>
+  </si>
+  <si>
+    <t>ngocnhu@gmail.com</t>
+  </si>
+  <si>
+    <t>Lê Ngọc Như</t>
+  </si>
+  <si>
+    <t>https://thao68.com/wp-content/uploads/2022/03/avatar-facebook-3.jpg</t>
   </si>
 </sst>
 </file>
@@ -818,9 +851,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1103,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,6 +2176,94 @@
         <v>191</v>
       </c>
     </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23">
+        <v>346494851</v>
+      </c>
+      <c r="F23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G23" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" t="s">
+        <v>205</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="2">
+        <v>37011</v>
+      </c>
+      <c r="K23" t="s">
+        <v>109</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24">
+        <v>366995813</v>
+      </c>
+      <c r="F24" t="s">
+        <v>192</v>
+      </c>
+      <c r="G24" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" t="s">
+        <v>210</v>
+      </c>
+      <c r="I24" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24" s="2">
+        <v>37001</v>
+      </c>
+      <c r="K24" t="s">
+        <v>110</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
fix error init db
</commit_message>
<xml_diff>
--- a/src/models/data/staff.xlsx
+++ b/src/models/data/staff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindonut\Documents\GitHub\Final\MEDRE_BE\src\models\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2193247-5899-484D-A349-113EF00968BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139BD3CD-54D9-410B-8CF0-8A30EB5CC120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="215">
   <si>
     <t>email</t>
   </si>
@@ -672,6 +672,15 @@
     <t>a12bc102-bab0-409e-9290-28320bea22ee</t>
   </si>
   <si>
+    <t>skied</t>
+  </si>
+  <si>
+    <t>0ba32cd2-e617-418a-84a0-9e53826a0b9d</t>
+  </si>
+  <si>
+    <t>transang123@gmail.com</t>
+  </si>
+  <si>
     <t>9edbd47a-186b-4c5b-a077-8446b7418f6f</t>
   </si>
   <si>
@@ -699,6 +708,9 @@
     <t>Lê Ngọc Như</t>
   </si>
   <si>
+    <t>https://thao68.com/wp-content/uploads/2022/03/avatar-facebook-3.jpg</t>
+  </si>
+  <si>
     <t>0968549326</t>
   </si>
   <si>
@@ -711,73 +723,76 @@
     <t>0863547861</t>
   </si>
   <si>
+    <t>0375435422</t>
+  </si>
+  <si>
     <t>0346494851</t>
   </si>
   <si>
     <t>0366995813</t>
   </si>
   <si>
+    <t>https://avamd.com/wp-content/uploads/2018/03/dr-simzar-500x760.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2023/01/James-Skala-DDS.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Furqan-Tejani-MD.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2015/08/IMG_5828-608x760.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2018/03/ava-md-7723-60-507x760.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Dmitry-Khasak-MD.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2016/01/Licia_Work.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2018/03/KA-507x760.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/hamid-bamshad-rpa-c.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2018/06/Jenna2-628x760.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Trajko-Bojadzievski-MD-%E2%80%93-Brooklyn-Endocrinologist.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Jivko-Gueorguiev-DDS.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/David-Soltanpour-MD.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/rohit-farzala.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2023/06/Dr.-Mikhail-Fukshansky-MD.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2018/03/bernice-cohen-634x760.jpg</t>
+  </si>
+  <si>
+    <t>https://avamd.com/wp-content/uploads/2020/01/Aileen-headshot-608x760.jpg</t>
+  </si>
+  <si>
     <t>https://avamd.com/wp-content/uploads/2018/02/dr-ava-shamban.jpg</t>
   </si>
   <si>
-    <t>https://avamd.com/wp-content/uploads/2018/03/bernice-cohen-634x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2020/01/Aileen-headshot-608x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2015/08/IMG_5828-608x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2018/03/ava-md-7723-60-507x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2018/03/dr-simzar-500x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2018/06/Jenna2-628x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2018/03/KA-507x760.jpg</t>
-  </si>
-  <si>
-    <t>https://avamd.com/wp-content/uploads/2016/01/Licia_Work.jpg</t>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Yevgeniy-Eugene-Mikityanskiy-DO.jpg</t>
+  </si>
+  <si>
+    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Bogdan-Brajic.jpg</t>
   </si>
   <si>
     <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Svetlana-Pyatigorskaya-MD.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Furqan-Tejani-MD.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Dmitry-Khasak-MD.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/hamid-bamshad-rpa-c.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Trajko-Bojadzievski-MD-%E2%80%93-Brooklyn-Endocrinologist.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Jivko-Gueorguiev-DDS.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2023/01/James-Skala-DDS.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Bogdan-Brajic.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/Yevgeniy-Eugene-Mikityanskiy-DO.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/David-Soltanpour-MD.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2022/11/rohit-farzala.jpg</t>
-  </si>
-  <si>
-    <t>https://www.centurymedicaldental.com/wp-content/uploads/2023/06/Dr.-Mikhail-Fukshansky-MD.jpg</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -1322,7 +1337,7 @@
         <v>105</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -1363,7 +1378,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F5" t="s">
         <v>169</v>
@@ -1372,7 +1387,7 @@
         <v>114</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="I5" t="s">
         <v>95</v>
@@ -1422,7 +1437,7 @@
         <v>115</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="I6" t="s">
         <v>95</v>
@@ -1472,7 +1487,7 @@
         <v>106</v>
       </c>
       <c r="H7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -1522,7 +1537,7 @@
         <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="I8" t="s">
         <v>95</v>
@@ -1563,7 +1578,7 @@
         <v>83</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F9" t="s">
         <v>169</v>
@@ -1572,7 +1587,7 @@
         <v>117</v>
       </c>
       <c r="H9" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="I9" t="s">
         <v>95</v>
@@ -1613,7 +1628,7 @@
         <v>84</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F10" t="s">
         <v>169</v>
@@ -1622,7 +1637,7 @@
         <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
@@ -1672,7 +1687,7 @@
         <v>118</v>
       </c>
       <c r="H11" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="I11" t="s">
         <v>95</v>
@@ -1722,7 +1737,7 @@
         <v>108</v>
       </c>
       <c r="H12" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
@@ -1772,7 +1787,7 @@
         <v>109</v>
       </c>
       <c r="H13" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="I13" t="s">
         <v>10</v>
@@ -1816,7 +1831,7 @@
         <v>110</v>
       </c>
       <c r="H14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I14" t="s">
         <v>10</v>
@@ -1860,7 +1875,7 @@
         <v>111</v>
       </c>
       <c r="H15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I15" t="s">
         <v>10</v>
@@ -1904,7 +1919,7 @@
         <v>112</v>
       </c>
       <c r="H16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I16" t="s">
         <v>10</v>
@@ -1925,7 +1940,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1939,7 +1954,7 @@
         <v>91</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F17" t="s">
         <v>169</v>
@@ -1948,7 +1963,7 @@
         <v>119</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="I17" t="s">
         <v>95</v>
@@ -1969,7 +1984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1992,7 +2007,7 @@
         <v>120</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="I18" t="s">
         <v>95</v>
@@ -2013,7 +2028,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2036,7 +2051,7 @@
         <v>121</v>
       </c>
       <c r="H19" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="I19" t="s">
         <v>95</v>
@@ -2057,7 +2072,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2080,7 +2095,7 @@
         <v>113</v>
       </c>
       <c r="H20" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="I20" t="s">
         <v>10</v>
@@ -2101,7 +2116,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>173</v>
       </c>
@@ -2125,39 +2140,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" t="s">
         <v>174</v>
       </c>
-      <c r="B22" t="s">
-        <v>175</v>
-      </c>
       <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
         <v>176</v>
       </c>
-      <c r="D22" t="s">
-        <v>177</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F22" t="s">
         <v>169</v>
       </c>
       <c r="G22" t="s">
-        <v>178</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="I22" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="2">
-        <v>37011</v>
+      <c r="J22" t="s">
+        <v>23</v>
       </c>
       <c r="K22" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -2166,50 +2181,100 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="O22" t="s">
+        <v>141</v>
+      </c>
+      <c r="P22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" t="s">
         <v>179</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>180</v>
       </c>
-      <c r="C23" t="s">
-        <v>176</v>
-      </c>
-      <c r="D23" t="s">
-        <v>181</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F23" t="s">
         <v>169</v>
       </c>
       <c r="G23" t="s">
+        <v>181</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2">
+        <v>37011</v>
+      </c>
+      <c r="K23" t="s">
+        <v>103</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>182</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F24" t="s">
+        <v>169</v>
+      </c>
+      <c r="G24" t="s">
+        <v>185</v>
+      </c>
+      <c r="H24" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" t="s">
         <v>95</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="2">
         <v>37001</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K24" t="s">
         <v>104</v>
       </c>
-      <c r="L23" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2217,12 +2282,12 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{302FE3D0-BB18-404B-81DE-91BA2AA6FC90}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{97E28657-8B9B-454E-A16D-780932F33430}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{61C2647B-81DD-45BA-9304-3607698ED2DD}"/>
-    <hyperlink ref="H17" r:id="rId4" xr:uid="{33775401-0228-4D14-AE8A-717A26E5A038}"/>
-    <hyperlink ref="H18" r:id="rId5" xr:uid="{E7490170-54F7-4E01-9658-CB2DA71CEB4C}"/>
-    <hyperlink ref="H23" r:id="rId6" xr:uid="{78E53992-DE4A-45EE-8152-912E3C94060B}"/>
-    <hyperlink ref="H2" r:id="rId7" xr:uid="{F8A41133-9AEE-46CC-AE64-9775D15815E2}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{699CA74D-67A2-439E-87AD-A0F9BBFF8D30}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{B383CACE-3734-48CE-ABD4-8869078669E4}"/>
+    <hyperlink ref="H17" r:id="rId4" xr:uid="{18C8432C-9B2C-4839-955F-D7B3DF5A9353}"/>
+    <hyperlink ref="H18" r:id="rId5" xr:uid="{6BF63A4D-9F31-4D71-95FB-CF883777EC20}"/>
+    <hyperlink ref="H23" r:id="rId6" xr:uid="{FCE4F019-0908-4951-A759-888F6846CF8A}"/>
+    <hyperlink ref="H2" r:id="rId7" xr:uid="{3DD417BB-02E7-45A0-978C-7F5BED06E77B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>